<commit_message>
relabel W36662 as non-producer & redo analysis
</commit_message>
<xml_diff>
--- a/data/rhamnolipids/rhamnMat.xlsx
+++ b/data/rhamnolipids/rhamnMat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liaoc/Documents/Source_code_for_Pseudomonas_Metabolomics_Paper/data/rhamnolipids/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18CABEA-A701-2B4A-9D89-B4FE8B876C85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA62F17-0D19-0444-8E7C-00A2C1D7137B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20300" yWindow="1020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rhamnMat_corrected" sheetId="1" r:id="rId1"/>
@@ -965,7 +965,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1250,10 +1250,10 @@
         <v>19</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>